<commit_message>
Refactoring code Inventory Adjustment and Cleaning code
</commit_message>
<xml_diff>
--- a/Import/Configurations/group_menu_template.xlsx
+++ b/Import/Configurations/group_menu_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\McDermott\Git\Import\Configurations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT Repositories\McDermott\Import\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B1D0CE-92AC-4191-89AC-08D14902A5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190B5741-C2DF-4D13-8E76-2DFCD9406251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Mandatory</t>
         </r>
@@ -43,7 +43,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Mandatory</t>
         </r>
@@ -55,7 +55,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Select one: Yes/No</t>
         </r>
@@ -67,7 +67,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Select one: Yes/No</t>
         </r>
@@ -79,7 +79,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Select one: Yes/No</t>
         </r>
@@ -91,7 +91,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Select one: Yes/No</t>
         </r>
@@ -103,7 +103,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Select one: Yes/No</t>
         </r>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="106">
   <si>
     <t>Menu</t>
   </si>
@@ -140,15 +140,9 @@
     <t>General Consultation Services</t>
   </si>
   <si>
-    <t>Clinic Service</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Medical Checkups</t>
-  </si>
-  <si>
     <t>Procedure Rooms</t>
   </si>
   <si>
@@ -158,24 +152,12 @@
     <t>Telemedicine</t>
   </si>
   <si>
-    <t>Accidents</t>
-  </si>
-  <si>
-    <t>Maternities</t>
-  </si>
-  <si>
-    <t>Wellness</t>
-  </si>
-  <si>
     <t>Reporting And Analytics</t>
   </si>
   <si>
     <t>Queue Counters</t>
   </si>
   <si>
-    <t xml:space="preserve">Queue </t>
-  </si>
-  <si>
     <t>Queue Displays</t>
   </si>
   <si>
@@ -191,9 +173,6 @@
     <t>BPJS Classifications</t>
   </si>
   <si>
-    <t>BPJS</t>
-  </si>
-  <si>
     <t>System Parameters</t>
   </si>
   <si>
@@ -236,9 +215,6 @@
     <t>Insurance Policies</t>
   </si>
   <si>
-    <t>Disease History</t>
-  </si>
-  <si>
     <t>Prescriptions</t>
   </si>
   <si>
@@ -323,9 +299,6 @@
     <t>Practitioners</t>
   </si>
   <si>
-    <t>Medical</t>
-  </si>
-  <si>
     <t>Doctor Schedules</t>
   </si>
   <si>
@@ -368,9 +341,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>Configuration</t>
-  </si>
-  <si>
     <t>Groups</t>
   </si>
   <si>
@@ -410,13 +380,58 @@
     <t>Chronic Diagnoses</t>
   </si>
   <si>
-    <t>Education Program</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>Stock Moves</t>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Medical Service</t>
+  </si>
+  <si>
+    <t>Medical Check up</t>
+  </si>
+  <si>
+    <t>Accidents Management</t>
+  </si>
+  <si>
+    <t>Maternity Check up</t>
+  </si>
+  <si>
+    <t>Diseases History</t>
+  </si>
+  <si>
+    <t>Benefit Configuration</t>
+  </si>
+  <si>
+    <t>Claim Management</t>
+  </si>
+  <si>
+    <t>Claim Request</t>
+  </si>
+  <si>
+    <t>Education &amp; Awareness Program</t>
+  </si>
+  <si>
+    <t>Education &amp; Awareness</t>
+  </si>
+  <si>
+    <t>Wellness Program</t>
+  </si>
+  <si>
+    <t>Wellness Management</t>
+  </si>
+  <si>
+    <t>BPJS Integrations</t>
+  </si>
+  <si>
+    <t>Medical Configurations</t>
+  </si>
+  <si>
+    <t>Report &amp; Analytic</t>
+  </si>
+  <si>
+    <t>System Configuration</t>
   </si>
 </sst>
 </file>
@@ -433,32 +448,26 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505021"/>
-        <bgColor theme="0" tint="-0.14996795556505021"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -488,15 +497,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +525,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table" displayName="Table" ref="A1:G86" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table" displayName="Table" ref="A1:G88" headerRowCount="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Menu"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Parent Menu"/>
@@ -787,19 +797,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -827,531 +839,531 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
-        <v>28</v>
-      </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1359,22 +1371,22 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1382,206 +1394,206 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1589,1195 +1601,1241 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="5" t="s">
-        <v>100</v>
+      <c r="A49" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="2" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="2" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="2" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="3" t="s">
-        <v>85</v>
+      <c r="A72" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="3" t="s">
-        <v>87</v>
+      <c r="A74" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="2" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="3" t="s">
-        <v>89</v>
+      <c r="A76" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="3" t="s">
-        <v>91</v>
+      <c r="A78" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="3" t="s">
-        <v>93</v>
+      <c r="A80" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="3" t="s">
-        <v>95</v>
+      <c r="A82" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>9</v>
+      <c r="A83" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F84" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G86" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>105</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>105</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>